<commit_message>
Source city selection from Excel
</commit_message>
<xml_diff>
--- a/billpay.xlsx
+++ b/billpay.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19001"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Selenium\IEOPeratorWillpay\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="21075" windowHeight="9975"/>
   </bookViews>
@@ -11,12 +16,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="45">
   <si>
     <t>Starting Date</t>
   </si>
@@ -37,24 +42,130 @@
   </si>
   <si>
     <t>y</t>
+  </si>
+  <si>
+    <t>http://cepatexpress.eticketing.my/Main/Login.asp</t>
+  </si>
+  <si>
+    <t>catchthatbus</t>
+  </si>
+  <si>
+    <t>cepat1234</t>
+  </si>
+  <si>
+    <t>http://ssinternational.eticketing.my/Main/Login.asp</t>
+  </si>
+  <si>
+    <t>ssi1096</t>
+  </si>
+  <si>
+    <t>http://megajaya.eticketing.my/Main/Login.asp</t>
+  </si>
+  <si>
+    <t>CTB KL AIMAN</t>
+  </si>
+  <si>
+    <t>mega2764</t>
+  </si>
+  <si>
+    <t>http://perdana.eticketing.my/Main/Login.asp</t>
+  </si>
+  <si>
+    <t>perdana283</t>
+  </si>
+  <si>
+    <t>http://prisma.eticketing.my/Main/Login.asp</t>
+  </si>
+  <si>
+    <t>azhar</t>
+  </si>
+  <si>
+    <t>pri62285</t>
+  </si>
+  <si>
+    <t>http://queen.eticketing.my/Main/Login.asp</t>
+  </si>
+  <si>
+    <t>CTB</t>
+  </si>
+  <si>
+    <t>qe56349</t>
+  </si>
+  <si>
+    <t>http://kesatuan.eticketing.my/Main/Login.asp</t>
+  </si>
+  <si>
+    <t>Ctb</t>
+  </si>
+  <si>
+    <t>ek5592</t>
+  </si>
+  <si>
+    <t>http://maju.eticketing.my/main/login.asp</t>
+  </si>
+  <si>
+    <t>zainab</t>
+  </si>
+  <si>
+    <t>maju5055</t>
+  </si>
+  <si>
+    <t>http://srimaju.eticketing.my/main/login.asp</t>
+  </si>
+  <si>
+    <t>CATCH</t>
+  </si>
+  <si>
+    <t>sm5055</t>
+  </si>
+  <si>
+    <t>http://quickliner.eticketing.my/Main/Login.asp</t>
+  </si>
+  <si>
+    <t>AZHAR</t>
+  </si>
+  <si>
+    <t>qle5055</t>
+  </si>
+  <si>
+    <t>http://mutiara.eticketing.my/Main/Login.asp</t>
+  </si>
+  <si>
+    <t>viren</t>
+  </si>
+  <si>
+    <t>em5055</t>
+  </si>
+  <si>
+    <t>http://se.eticketing.my</t>
+  </si>
+  <si>
+    <t>ctb</t>
+  </si>
+  <si>
+    <t>see5055</t>
+  </si>
+  <si>
+    <t>http://13.76.85.166:114/Main/Login.asp</t>
+  </si>
+  <si>
+    <t>Pass1234</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>grik</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -77,19 +188,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -97,6 +206,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -145,7 +257,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -178,9 +290,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -213,6 +342,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -389,17 +535,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="44" customWidth="1"/>
-    <col min="2" max="2" width="30.85546875" customWidth="1"/>
-    <col min="3" max="3" width="18.85546875" customWidth="1"/>
+    <col min="1" max="1" width="49.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="48.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -414,37 +562,398 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>43121</v>
+      </c>
+      <c r="B3" s="2">
+        <v>43122</v>
+      </c>
+      <c r="C3" s="1">
+        <f>DATEDIF(A3,B3,"d")</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="4">
-        <v>43115</v>
-      </c>
-      <c r="B3" s="4">
-        <v>43120</v>
-      </c>
-      <c r="C3" s="2">
-        <f>DATEDIF(A3,B3,"d")</f>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>43135</v>
+      </c>
+      <c r="B5" s="2">
+        <v>43136</v>
+      </c>
+      <c r="C5" s="1">
+        <f>DATEDIF(A5,B5,"d")</f>
+        <v>1</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>43121</v>
+      </c>
+      <c r="B7" s="2">
+        <v>43122</v>
+      </c>
+      <c r="C7" s="1">
+        <f>DATEDIF(A7,B7,"d")</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>43128</v>
+      </c>
+      <c r="B9" s="2">
+        <v>43129</v>
+      </c>
+      <c r="C9" s="1">
+        <f>DATEDIF(A9,B9,"d")</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>43121</v>
+      </c>
+      <c r="B11" s="2">
+        <v>43122</v>
+      </c>
+      <c r="C11" s="1">
+        <f>DATEDIF(A11,B11,"d")</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>43121</v>
+      </c>
+      <c r="B13" s="2">
+        <v>43122</v>
+      </c>
+      <c r="C13" s="1">
+        <f>DATEDIF(A13,B13,"d")</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <v>43121</v>
+      </c>
+      <c r="B15" s="2">
+        <v>43122</v>
+      </c>
+      <c r="C15" s="1">
+        <f>DATEDIF(A15,B15,"d")</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>43121</v>
+      </c>
+      <c r="B17" s="2">
+        <v>43122</v>
+      </c>
+      <c r="C17" s="1">
+        <f>DATEDIF(A17,B17,"d")</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
+        <v>43121</v>
+      </c>
+      <c r="B19" s="2">
+        <v>43122</v>
+      </c>
+      <c r="C19" s="1">
+        <f>DATEDIF(A19,B19,"d")</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
+        <v>43121</v>
+      </c>
+      <c r="B21" s="2">
+        <v>43122</v>
+      </c>
+      <c r="C21" s="1">
+        <f>DATEDIF(A21,B21,"d")</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C22" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="2"/>
+      <c r="D22" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
+        <v>43121</v>
+      </c>
+      <c r="B23" s="2">
+        <v>43122</v>
+      </c>
+      <c r="C23" s="1">
+        <f>DATEDIF(A23,B23,"d")</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="2">
+        <v>43121</v>
+      </c>
+      <c r="B25" s="2">
+        <v>43122</v>
+      </c>
+      <c r="C25" s="1">
+        <f>DATEDIF(A25,B25,"d")</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="2">
+        <v>43121</v>
+      </c>
+      <c r="B27" s="2">
+        <v>43122</v>
+      </c>
+      <c r="C27" s="1">
+        <f>DATEDIF(A27,B27,"d")</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="2">
+        <v>43121</v>
+      </c>
+      <c r="B29" s="2">
+        <v>43122</v>
+      </c>
+      <c r="C29" s="1">
+        <f>DATEDIF(A29,B29,"d")</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="2">
+        <v>43121</v>
+      </c>
+      <c r="B31" s="2">
+        <v>43122</v>
+      </c>
+      <c r="C31" s="1">
+        <f>DATEDIF(A31,B31,"d")</f>
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>